<commit_message>
Updated title of table column
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denniszomar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B65B3A0-6B22-6F49-8A1A-2CEB56321E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ED4805-D394-4142-A27D-26491BF89611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{476524D5-AEB5-914C-AC2D-37EF6F8911B3}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>CA</t>
   </si>
   <si>
-    <t>TimeSpent</t>
-  </si>
-  <si>
     <t>Work</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Fishtown</t>
+  </si>
+  <si>
+    <t>Time Spent</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,7 +535,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -860,13 +860,13 @@
         <v>-75.136912695684103</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" t="s">
         <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>0.5</v>
@@ -892,10 +892,10 @@
         <v>2.125</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -915,10 +915,10 @@
         <v>6</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -929,7 +929,7 @@
         <v>-159.78291495236999</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>24</v>
@@ -938,10 +938,10 @@
         <v>2.33</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -952,7 +952,7 @@
         <v>-71.139871658776897</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>23</v>
@@ -961,10 +961,10 @@
         <v>3.5</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -975,19 +975,19 @@
         <v>-74.901727264659797</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F21" s="1">
         <v>0.5</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted table column name and added short name
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denniszomar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ED4805-D394-4142-A27D-26491BF89611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8277C45-CE27-5349-9382-42FA2E19A615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{476524D5-AEB5-914C-AC2D-37EF6F8911B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>Latitude</t>
   </si>
@@ -149,7 +149,19 @@
     <t>Fishtown</t>
   </si>
   <si>
-    <t>Time Spent</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TimeSpent</t>
+  </si>
+  <si>
+    <t>CSEDS</t>
+  </si>
+  <si>
+    <t>Marlboro</t>
+  </si>
+  <si>
+    <t>Canal Street</t>
   </si>
 </sst>
 </file>
@@ -185,9 +197,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399E871-1860-C446-9F3F-B5E63098A62F}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,478 +527,529 @@
     <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>42.323406956946997</v>
+      </c>
+      <c r="B2">
+        <v>-71.112516825936893</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>1.25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>42.393875477651498</v>
+      </c>
+      <c r="B3">
+        <v>-71.111492974932304</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>1.75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>42.348119765585402</v>
+      </c>
+      <c r="B4">
+        <v>-71.079645396421796</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>1.75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>42.365346409545502</v>
+      </c>
+      <c r="B5">
+        <v>-71.056391908667706</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>42.336742056755099</v>
+      </c>
+      <c r="B6">
+        <v>-71.097566157743103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>42.331524215120602</v>
+      </c>
+      <c r="B7">
+        <v>-71.104229522470803</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>21.8875989842048</v>
+      </c>
+      <c r="B8">
+        <v>-159.477291299538</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>21.869374334332299</v>
+      </c>
+      <c r="B9">
+        <v>-159.44600064927701</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>0.33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>42.373999852375597</v>
+      </c>
+      <c r="B10">
+        <v>-71.519369337907904</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>42.704232885108297</v>
+      </c>
+      <c r="B11">
+        <v>-71.576506319685805</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>1.75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>42.841975326816097</v>
+      </c>
+      <c r="B12">
+        <v>-71.638983295159704</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>1.25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>42.761025887835103</v>
+      </c>
+      <c r="B13">
+        <v>-71.470520458268794</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>42.323406956946997</v>
-      </c>
-      <c r="B2" s="1">
-        <v>-71.112516825936893</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>42.393875477651498</v>
-      </c>
-      <c r="B3" s="1">
-        <v>-71.111492974932304</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>42.348119765585402</v>
-      </c>
-      <c r="B4" s="1">
-        <v>-71.079645396421796</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>42.365346409545502</v>
-      </c>
-      <c r="B5" s="1">
-        <v>-71.056391908667706</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>42.336742056755099</v>
-      </c>
-      <c r="B6" s="1">
-        <v>-71.097566157743103</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>42.331524215120602</v>
-      </c>
-      <c r="B7" s="1">
-        <v>-71.104229522470803</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>21.8875989842048</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-159.477291299538</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>21.869374334332299</v>
-      </c>
-      <c r="B9" s="1">
-        <v>-159.44600064927701</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>42.373999852375597</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-71.519369337907904</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>42.704232885108297</v>
-      </c>
-      <c r="B11" s="1">
-        <v>-71.576506319685805</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>42.841975326816097</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-71.638983295159704</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>42.761025887835103</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-71.470520458268794</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>33.878721128042102</v>
       </c>
       <c r="B14">
         <v>-118.357016964804</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>2</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>35.033736026932303</v>
       </c>
       <c r="B15">
         <v>-120.529843039677</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>4</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39.973793002173799</v>
       </c>
       <c r="B16">
         <v>-75.136912695684103</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>35</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>0.5</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>42.347562118574103</v>
       </c>
       <c r="B17">
         <v>-71.489319839498293</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>2.125</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>42.763678418910402</v>
       </c>
       <c r="B18">
         <v>-71.458378098993293</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>22.0500700284543</v>
       </c>
       <c r="B19">
         <v>-159.78291495236999</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>2.33</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>42.521241785380298</v>
       </c>
       <c r="B20">
         <v>-71.139871658776897</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>3.5</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>39.979907863295097</v>
       </c>
       <c r="B21">
         <v>-74.901727264659797</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>0.5</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>